<commit_message>
something is very wrong with the script!
</commit_message>
<xml_diff>
--- a/TESTING.xlsx
+++ b/TESTING.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,71 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.bing.com/</t>
+          <t>https://www.imdb.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>True - Redirect</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>&lt;button id="suggestion-search-button" type="submit" aria-label="Submit Search" class="nav-search__search-submit searchform__submit"&gt;&lt;svg xmlns="http://www.w3.org/2000/svg" width="24" height="24" class="ipc-icon ipc-icon--magnify" viewBox="0 0 24 24" fill="currentColor" role="presentation"&gt;&lt;path fill="none" d="M0 0h24v24H0V0z"&gt;&lt;/path&gt;&lt;path d="M15.5 14h-.79l-.28-.27a6.5 6.5 0 0 0 1.48-5.34c-.47-2.78-2.79-5-5.59-5.34a6.505 6.505 0 0 0-7.27 7.27c.34 2.8 2.56 5.12 5.34 5.59a6.5 6.5 0 0 0 5.34-1.48l.27.28v.79l4.25 4.25c.41.41 1.08.41 1.49 0 .41-.41.41-1.08 0-1.49L15.5 14zm-6 0C7.01 14 5 11.99 5 9.5S7.01 5 9.5 5 14 7.01 14 9.5 11.99 14 9.5 14z"&gt;&lt;/path&gt;&lt;/svg&gt;&lt;/button&gt;</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Tries: 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>True - Redirect</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>&lt;a data-testid="wtw-button" class="ipc-btn ipc-btn--single-padding ipc-btn--center-align-content ipc-btn--default-height ipc-btn--core-baseAlt ipc-btn--theme-baseAlt ipc-btn--on-accent2 ipc-text-button sc-78fcd8c-2 cWpSXA" role="button" tabindex="0" aria-disabled="false" href="/what-to-watch?ref_=hm_watch_btn"&gt;&lt;span class="ipc-btn__text"&gt;Get more recommendations&lt;/span&gt;&lt;svg xmlns="http://www.w3.org/2000/svg" width="24" height="24" class="ipc-icon ipc-icon--chevron-right ipc-btn__icon ipc-btn__icon--post" viewBox="0 0 24 24" fill="currentColor" role="presentation"&gt;&lt;path fill="none" d="M0 0h24v24H0V0z"&gt;&lt;/path&gt;&lt;path d="M9.29 6.71a.996.996 0 0 0 0 1.41L13.17 12l-3.88 3.88a.996.996 0 1 0 1.41 1.41l4.59-4.59a.996.996 0 0 0 0-1.41L10.7 6.7c-.38-.38-1.02-.38-1.41.01z"&gt;&lt;/path&gt;&lt;/svg&gt;&lt;/a&gt;</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Tries: 1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
VERY GOOD WORK TODAY !
</commit_message>
<xml_diff>
--- a/TESTING.xlsx
+++ b/TESTING.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,20 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Main_Page</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>testing 15 / 15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>